<commit_message>
Add per-shot information to results
</commit_message>
<xml_diff>
--- a/estimating-tds/results.xlsx
+++ b/estimating-tds/results.xlsx
@@ -3,27 +3,52 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="samples" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="trials" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="oven_times" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="tubes" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="samples" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="trials" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="oven_times" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>tube_id</t>
+    <t>coffee</t>
   </si>
   <si>
-    <t>coffee</t>
+    <t>weight_in</t>
+  </si>
+  <si>
+    <t>weight_out</t>
+  </si>
+  <si>
+    <t>shot_time</t>
+  </si>
+  <si>
+    <t>temp_at_group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Doppelganger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roselis Herrera</t>
+  </si>
+  <si>
+    <t>Rukira</t>
+  </si>
+  <si>
+    <t>tube_id</t>
   </si>
   <si>
     <t>filtered</t>
@@ -32,28 +57,7 @@
     <t>filtrate_weight</t>
   </si>
   <si>
-    <t>1A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Doppelganger</t>
-  </si>
-  <si>
     <t>no</t>
-  </si>
-  <si>
-    <t>2A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Standard</t>
-  </si>
-  <si>
-    <t>3A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roselis Herrera</t>
-  </si>
-  <si>
-    <t>Rukira</t>
   </si>
   <si>
     <t>yes</t>
@@ -162,11 +166,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="160" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1">
     <font>
+      <sz val="11.000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <color theme="1"/>
-      <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -190,13 +197,19 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="21" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -712,6 +725,507 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
+    <col min="4" max="5" style="1" width="9.140625"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="5">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2">
+        <v>41.700000000000003</v>
+      </c>
+      <c r="E2" s="3">
+        <v>37</v>
+      </c>
+      <c r="F2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2">
+        <v>40.899999999999999</v>
+      </c>
+      <c r="E3" s="6">
+        <v>36</v>
+      </c>
+      <c r="F3" s="4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="E4" s="3">
+        <v>34</v>
+      </c>
+      <c r="F4">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5">
+        <v>19</v>
+      </c>
+      <c r="D5" s="2">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="E5" s="6">
+        <v>36</v>
+      </c>
+      <c r="F5" s="4">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2">
+        <v>40.100000000000001</v>
+      </c>
+      <c r="E6" s="3">
+        <v>31</v>
+      </c>
+      <c r="F6">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="5">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="E7" s="6">
+        <v>31</v>
+      </c>
+      <c r="F7" s="4">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="5">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2">
+        <v>41.399999999999999</v>
+      </c>
+      <c r="E8" s="3">
+        <v>33</v>
+      </c>
+      <c r="F8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2">
+        <v>40</v>
+      </c>
+      <c r="E9" s="3">
+        <v>31</v>
+      </c>
+      <c r="F9">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="5">
+        <v>19</v>
+      </c>
+      <c r="D10" s="2">
+        <v>40.100000000000001</v>
+      </c>
+      <c r="E10" s="3">
+        <v>30</v>
+      </c>
+      <c r="F10">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="5">
+        <v>19</v>
+      </c>
+      <c r="D11" s="2">
+        <v>41</v>
+      </c>
+      <c r="E11" s="6">
+        <v>35</v>
+      </c>
+      <c r="F11" s="4">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="5">
+        <v>19</v>
+      </c>
+      <c r="D12" s="2">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="E12" s="6">
+        <v>35</v>
+      </c>
+      <c r="F12" s="4">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="5">
+        <v>19</v>
+      </c>
+      <c r="D13" s="2">
+        <v>41.299999999999997</v>
+      </c>
+      <c r="E13" s="6">
+        <v>34</v>
+      </c>
+      <c r="F13" s="4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="5">
+        <v>19</v>
+      </c>
+      <c r="D14" s="2">
+        <v>41.600000000000001</v>
+      </c>
+      <c r="E14" s="6">
+        <v>33</v>
+      </c>
+      <c r="F14" s="4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="5">
+        <v>19</v>
+      </c>
+      <c r="D15" s="2">
+        <v>42.700000000000003</v>
+      </c>
+      <c r="E15" s="3">
+        <v>31</v>
+      </c>
+      <c r="F15">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="5">
+        <v>19</v>
+      </c>
+      <c r="D16" s="2">
+        <v>43</v>
+      </c>
+      <c r="E16" s="3">
+        <v>34</v>
+      </c>
+      <c r="F16">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="5">
+        <v>19</v>
+      </c>
+      <c r="D17" s="2">
+        <v>41.399999999999999</v>
+      </c>
+      <c r="E17" s="3">
+        <v>34</v>
+      </c>
+      <c r="F17">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="5">
+        <v>19</v>
+      </c>
+      <c r="D18" s="2">
+        <v>41.899999999999999</v>
+      </c>
+      <c r="E18" s="3">
+        <v>38</v>
+      </c>
+      <c r="F18">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="5">
+        <v>19</v>
+      </c>
+      <c r="D19" s="2">
+        <v>41.200000000000003</v>
+      </c>
+      <c r="E19" s="3">
+        <v>33</v>
+      </c>
+      <c r="F19">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="5">
+        <v>19</v>
+      </c>
+      <c r="D20" s="2">
+        <v>40.399999999999999</v>
+      </c>
+      <c r="E20" s="3">
+        <v>32</v>
+      </c>
+      <c r="F20">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="5">
+        <v>19</v>
+      </c>
+      <c r="D21" s="2">
+        <v>41.5</v>
+      </c>
+      <c r="E21" s="3">
+        <v>33</v>
+      </c>
+      <c r="F21">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="5">
+        <v>19</v>
+      </c>
+      <c r="D22" s="2">
+        <v>40.5</v>
+      </c>
+      <c r="E22" s="3">
+        <v>32</v>
+      </c>
+      <c r="F22">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="5">
+        <v>19</v>
+      </c>
+      <c r="D23" s="2">
+        <v>41</v>
+      </c>
+      <c r="E23" s="3">
+        <v>34</v>
+      </c>
+      <c r="F23">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="5">
+        <v>19</v>
+      </c>
+      <c r="D24" s="2">
+        <v>40.899999999999999</v>
+      </c>
+      <c r="E24" s="3">
+        <v>34</v>
+      </c>
+      <c r="F24">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25"/>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
     <col customWidth="1" min="3" max="4" width="9.140625"/>
   </cols>
   <sheetData>
@@ -719,59 +1233,59 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+      <c r="D1" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
+      <c r="B2">
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
+      <c r="B3">
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
+      <c r="B4">
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" ht="14.25">
@@ -779,78 +1293,78 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="2">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
+      <c r="B6">
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6">
         <v>17.190000000000001</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="2">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
+      <c r="B7">
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7">
         <v>21.390000000000001</v>
       </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="2">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>10</v>
+      <c r="B8">
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E8">
         <v>19.82</v>
       </c>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="2">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E9">
         <v>15.93</v>
@@ -860,11 +1374,11 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>7</v>
+      <c r="C10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" ht="14.25">
@@ -878,7 +1392,7 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" ht="14.25">
@@ -889,10 +1403,10 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" ht="14.25">
@@ -903,10 +1417,10 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" ht="14.25">
@@ -917,10 +1431,10 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" ht="14.25">
@@ -934,7 +1448,7 @@
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E15">
         <v>17.120000000000001</v>
@@ -948,10 +1462,10 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E16">
         <v>14.140000000000001</v>
@@ -965,10 +1479,10 @@
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E17">
         <v>17.77</v>
@@ -982,10 +1496,10 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E18">
         <v>18.27</v>
@@ -1002,9 +1516,9 @@
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" ht="14.25">
       <c r="A20">
@@ -1014,12 +1528,12 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" ht="14.25">
       <c r="A21">
@@ -1029,12 +1543,12 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="E21" s="4"/>
     </row>
     <row r="22" ht="14.25">
       <c r="A22">
@@ -1044,12 +1558,12 @@
         <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="E22" s="4"/>
     </row>
     <row r="23" ht="14.25">
       <c r="A23">
@@ -1062,9 +1576,9 @@
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="2">
+        <v>14</v>
+      </c>
+      <c r="E23" s="4">
         <v>19.989999999999998</v>
       </c>
     </row>
@@ -1076,12 +1590,12 @@
         <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="2">
+        <v>14</v>
+      </c>
+      <c r="E24" s="4">
         <v>19.690000000000001</v>
       </c>
     </row>
@@ -1093,12 +1607,12 @@
         <v>20</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="2">
+        <v>14</v>
+      </c>
+      <c r="E25" s="4">
         <v>19.899999999999999</v>
       </c>
     </row>
@@ -1110,24 +1624,24 @@
         <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="2">
+        <v>14</v>
+      </c>
+      <c r="E26" s="4">
         <v>19.309999999999999</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView topLeftCell="A34" zoomScale="100" workbookViewId="0">
@@ -1144,58 +1658,58 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="N1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="O1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="P1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="Q1" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R1" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="S1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" ht="14.25">
@@ -1211,13 +1725,13 @@
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
         <v>19.5</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="4">
         <v>1.3329899999999999</v>
       </c>
       <c r="H2">
@@ -1238,19 +1752,19 @@
       <c r="M2">
         <v>1.34846</v>
       </c>
-      <c r="N2" s="1">
+      <c r="N2" s="7">
         <v>2.214</v>
       </c>
-      <c r="O2" s="1">
+      <c r="O2" s="7">
         <v>2.21</v>
       </c>
-      <c r="P2" s="1">
+      <c r="P2" s="7">
         <v>2.21</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="Q2" s="7">
         <v>2.2189999999999999</v>
       </c>
-      <c r="R2" s="1">
+      <c r="R2" s="7">
         <v>2.2229999999999999</v>
       </c>
     </row>
@@ -1267,13 +1781,13 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
         <v>19</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="4">
         <v>1.3329899999999999</v>
       </c>
       <c r="H3">
@@ -1294,19 +1808,19 @@
       <c r="M3">
         <v>1.3482000000000001</v>
       </c>
-      <c r="N3" s="1">
+      <c r="N3" s="7">
         <v>2.1659999999999999</v>
       </c>
-      <c r="O3" s="1">
+      <c r="O3" s="7">
         <v>2.1629999999999998</v>
       </c>
-      <c r="P3" s="1">
+      <c r="P3" s="7">
         <v>2.1640000000000001</v>
       </c>
-      <c r="Q3" s="1">
+      <c r="Q3" s="7">
         <v>2.1699999999999999</v>
       </c>
-      <c r="R3" s="1">
+      <c r="R3" s="7">
         <v>2.177</v>
       </c>
     </row>
@@ -1323,13 +1837,13 @@
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
         <v>18.800000000000001</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="4">
         <v>1.3329899999999999</v>
       </c>
       <c r="H4">
@@ -1350,19 +1864,19 @@
       <c r="M4">
         <v>1.3488599999999999</v>
       </c>
-      <c r="N4" s="1">
+      <c r="N4" s="7">
         <v>2.254</v>
       </c>
-      <c r="O4" s="1">
+      <c r="O4" s="7">
         <v>2.2519999999999998</v>
       </c>
-      <c r="P4" s="1">
+      <c r="P4" s="7">
         <v>2.2509999999999999</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="Q4" s="7">
         <v>2.258</v>
       </c>
-      <c r="R4" s="1">
+      <c r="R4" s="7">
         <v>2.2639999999999998</v>
       </c>
     </row>
@@ -1379,13 +1893,13 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
         <v>19</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="4">
         <v>1.3329899999999999</v>
       </c>
       <c r="H5">
@@ -1406,19 +1920,19 @@
       <c r="M5">
         <v>1.34894</v>
       </c>
-      <c r="N5" s="1">
+      <c r="N5" s="7">
         <v>2.2679999999999998</v>
       </c>
-      <c r="O5" s="1">
+      <c r="O5" s="7">
         <v>2.2650000000000001</v>
       </c>
-      <c r="P5" s="1">
+      <c r="P5" s="7">
         <v>2.2639999999999998</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="Q5" s="7">
         <v>2.2719999999999998</v>
       </c>
-      <c r="R5" s="1">
+      <c r="R5" s="7">
         <v>2.2770000000000001</v>
       </c>
     </row>
@@ -1462,19 +1976,19 @@
       <c r="M6">
         <v>1.3464499999999999</v>
       </c>
-      <c r="N6" s="1">
+      <c r="N6" s="7">
         <v>1.857</v>
       </c>
-      <c r="O6" s="1">
+      <c r="O6" s="7">
         <v>1.857</v>
       </c>
-      <c r="P6" s="1">
+      <c r="P6" s="7">
         <v>1.855</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="Q6" s="7">
         <v>1.8620000000000001</v>
       </c>
-      <c r="R6" s="1">
+      <c r="R6" s="7">
         <v>1.867</v>
       </c>
     </row>
@@ -1518,19 +2032,19 @@
       <c r="M7">
         <v>1.3391500000000001</v>
       </c>
-      <c r="N7" s="1">
+      <c r="N7" s="7">
         <v>1.504</v>
       </c>
-      <c r="O7" s="1">
+      <c r="O7" s="7">
         <v>1.5049999999999999</v>
       </c>
-      <c r="P7" s="1">
+      <c r="P7" s="7">
         <v>1.5029999999999999</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="Q7" s="7">
         <v>1.5109999999999999</v>
       </c>
-      <c r="R7" s="1">
+      <c r="R7" s="7">
         <v>1.516</v>
       </c>
     </row>
@@ -1574,19 +2088,19 @@
       <c r="M8">
         <v>1.3354699999999999</v>
       </c>
-      <c r="N8" s="1">
+      <c r="N8" s="7">
         <v>1.302</v>
       </c>
-      <c r="O8" s="1">
+      <c r="O8" s="7">
         <v>1.3029999999999999</v>
       </c>
-      <c r="P8" s="1">
+      <c r="P8" s="7">
         <v>1.302</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="Q8" s="7">
         <v>1.3109999999999999</v>
       </c>
-      <c r="R8" s="1">
+      <c r="R8" s="7">
         <v>1.3140000000000001</v>
       </c>
     </row>
@@ -1630,19 +2144,19 @@
       <c r="M9">
         <v>1.3341000000000001</v>
       </c>
-      <c r="N9" s="1">
+      <c r="N9" s="7">
         <v>1.242</v>
       </c>
-      <c r="O9" s="1">
+      <c r="O9" s="7">
         <v>1.2430000000000001</v>
       </c>
-      <c r="P9" s="1">
+      <c r="P9" s="7">
         <v>1.242</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="Q9" s="7">
         <v>1.25</v>
       </c>
-      <c r="R9" s="1">
+      <c r="R9" s="7">
         <v>1.254</v>
       </c>
     </row>
@@ -1686,19 +2200,19 @@
       <c r="M10">
         <v>1.3333999999999999</v>
       </c>
-      <c r="N10" s="1">
+      <c r="N10" s="7">
         <v>1.212</v>
       </c>
-      <c r="O10" s="1">
+      <c r="O10" s="7">
         <v>1.21</v>
       </c>
-      <c r="P10" s="1">
+      <c r="P10" s="7">
         <v>1.2110000000000001</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="Q10" s="7">
         <v>1.2190000000000001</v>
       </c>
-      <c r="R10" s="1">
+      <c r="R10" s="7">
         <v>1.222</v>
       </c>
     </row>
@@ -1742,19 +2256,19 @@
       <c r="M11">
         <v>1.3465100000000001</v>
       </c>
-      <c r="N11" s="1">
+      <c r="N11" s="7">
         <v>1.8560000000000001</v>
       </c>
-      <c r="O11" s="1">
+      <c r="O11" s="7">
         <v>1.855</v>
       </c>
-      <c r="P11" s="1">
+      <c r="P11" s="7">
         <v>1.8540000000000001</v>
       </c>
-      <c r="Q11" s="1">
+      <c r="Q11" s="7">
         <v>1.861</v>
       </c>
-      <c r="R11" s="1">
+      <c r="R11" s="7">
         <v>1.8660000000000001</v>
       </c>
     </row>
@@ -1798,19 +2312,19 @@
       <c r="M12">
         <v>1.33982</v>
       </c>
-      <c r="N12" s="1">
+      <c r="N12" s="7">
         <v>1.599</v>
       </c>
-      <c r="O12" s="1">
+      <c r="O12" s="7">
         <v>1.599</v>
       </c>
-      <c r="P12" s="1">
+      <c r="P12" s="7">
         <v>1.597</v>
       </c>
-      <c r="Q12" s="1">
+      <c r="Q12" s="7">
         <v>1.6040000000000001</v>
       </c>
-      <c r="R12" s="1">
+      <c r="R12" s="7">
         <v>1.6100000000000001</v>
       </c>
     </row>
@@ -1854,19 +2368,19 @@
       <c r="M13">
         <v>1.33656</v>
       </c>
-      <c r="N13" s="1">
+      <c r="N13" s="7">
         <v>1.3420000000000001</v>
       </c>
-      <c r="O13" s="1">
+      <c r="O13" s="7">
         <v>1.341</v>
       </c>
-      <c r="P13" s="1">
+      <c r="P13" s="7">
         <v>1.341</v>
       </c>
-      <c r="Q13" s="1">
+      <c r="Q13" s="7">
         <v>1.3480000000000001</v>
       </c>
-      <c r="R13" s="1">
+      <c r="R13" s="7">
         <v>1.3520000000000001</v>
       </c>
     </row>
@@ -1910,19 +2424,19 @@
       <c r="M14">
         <v>1.3347800000000001</v>
       </c>
-      <c r="N14" s="1">
+      <c r="N14" s="7">
         <v>1.25</v>
       </c>
-      <c r="O14" s="1">
+      <c r="O14" s="7">
         <v>1.2470000000000001</v>
       </c>
-      <c r="P14" s="1">
+      <c r="P14" s="7">
         <v>1.2470000000000001</v>
       </c>
-      <c r="Q14" s="1">
+      <c r="Q14" s="7">
         <v>1.254</v>
       </c>
-      <c r="R14" s="1">
+      <c r="R14" s="7">
         <v>1.2569999999999999</v>
       </c>
     </row>
@@ -1966,19 +2480,19 @@
       <c r="M15">
         <v>1.33392</v>
       </c>
-      <c r="N15" s="1">
+      <c r="N15" s="7">
         <v>1.25</v>
       </c>
-      <c r="O15" s="1">
+      <c r="O15" s="7">
         <v>1.2490000000000001</v>
       </c>
-      <c r="P15" s="1">
+      <c r="P15" s="7">
         <v>1.2490000000000001</v>
       </c>
-      <c r="Q15" s="1">
+      <c r="Q15" s="7">
         <v>1.258</v>
       </c>
-      <c r="R15" s="1">
+      <c r="R15" s="7">
         <v>1.2609999999999999</v>
       </c>
     </row>
@@ -2022,19 +2536,19 @@
       <c r="M16">
         <v>1.34534</v>
       </c>
-      <c r="N16" s="1">
+      <c r="N16" s="7">
         <v>1.7789999999999999</v>
       </c>
-      <c r="O16" s="1">
+      <c r="O16" s="7">
         <v>1.7769999999999999</v>
       </c>
-      <c r="P16" s="1">
+      <c r="P16" s="7">
         <v>1.7769999999999999</v>
       </c>
-      <c r="Q16" s="1">
+      <c r="Q16" s="7">
         <v>1.7829999999999999</v>
       </c>
-      <c r="R16" s="1">
+      <c r="R16" s="7">
         <v>1.788</v>
       </c>
     </row>
@@ -2078,30 +2592,30 @@
       <c r="M17">
         <v>1.3393999999999999</v>
       </c>
-      <c r="N17" s="1">
+      <c r="N17" s="7">
         <v>1.5549999999999999</v>
       </c>
-      <c r="O17" s="1">
+      <c r="O17" s="7">
         <v>1.5529999999999999</v>
       </c>
-      <c r="P17" s="1">
+      <c r="P17" s="7">
         <v>1.554</v>
       </c>
-      <c r="Q17" s="1">
+      <c r="Q17" s="7">
         <v>1.5600000000000001</v>
       </c>
-      <c r="R17" s="1">
+      <c r="R17" s="7">
         <v>1.5649999999999999</v>
       </c>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="2">
+      <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="4">
         <v>7</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="4">
         <v>1.21</v>
       </c>
       <c r="D18">
@@ -2128,29 +2642,29 @@
       <c r="K18">
         <v>0.79000000000000004</v>
       </c>
-      <c r="L18" s="2">
+      <c r="L18" s="4">
         <v>19.399999999999999</v>
       </c>
-      <c r="M18" s="2">
+      <c r="M18" s="4">
         <v>1.3343700000000001</v>
       </c>
-      <c r="N18" s="1">
+      <c r="N18" s="7">
         <v>1.29</v>
       </c>
-      <c r="O18" s="2">
+      <c r="O18" s="4">
         <v>1.288</v>
       </c>
-      <c r="P18" s="2">
+      <c r="P18" s="4">
         <v>1.288</v>
       </c>
-      <c r="Q18" s="2">
+      <c r="Q18" s="4">
         <v>1.296</v>
       </c>
-      <c r="R18" s="2">
+      <c r="R18" s="4">
         <v>1.3009999999999999</v>
       </c>
       <c r="S18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" ht="14.25">
@@ -2193,19 +2707,19 @@
       <c r="M19">
         <v>1.33585</v>
       </c>
-      <c r="N19" s="2">
+      <c r="N19" s="4">
         <v>1.371</v>
       </c>
-      <c r="O19" s="1">
+      <c r="O19" s="7">
         <v>1.371</v>
       </c>
-      <c r="P19" s="1">
+      <c r="P19" s="7">
         <v>1.3720000000000001</v>
       </c>
-      <c r="Q19" s="1">
+      <c r="Q19" s="7">
         <v>1.379</v>
       </c>
-      <c r="R19" s="1">
+      <c r="R19" s="7">
         <v>1.3819999999999999</v>
       </c>
     </row>
@@ -2249,19 +2763,19 @@
       <c r="M20">
         <v>1.33361</v>
       </c>
-      <c r="N20" s="1">
+      <c r="N20" s="7">
         <v>1.2390000000000001</v>
       </c>
-      <c r="O20" s="1">
+      <c r="O20" s="7">
         <v>1.236</v>
       </c>
-      <c r="P20" s="1">
+      <c r="P20" s="7">
         <v>1.238</v>
       </c>
-      <c r="Q20" s="1">
+      <c r="Q20" s="7">
         <v>1.2450000000000001</v>
       </c>
-      <c r="R20" s="1">
+      <c r="R20" s="7">
         <v>1.2470000000000001</v>
       </c>
     </row>
@@ -2305,19 +2819,19 @@
       <c r="M21">
         <v>1.34677</v>
       </c>
-      <c r="N21" s="1">
+      <c r="N21" s="7">
         <v>1.77</v>
       </c>
-      <c r="O21" s="1">
+      <c r="O21" s="7">
         <v>1.768</v>
       </c>
-      <c r="P21" s="1">
+      <c r="P21" s="7">
         <v>1.7669999999999999</v>
       </c>
-      <c r="Q21" s="1">
+      <c r="Q21" s="7">
         <v>1.774</v>
       </c>
-      <c r="R21" s="1">
+      <c r="R21" s="7">
         <v>1.778</v>
       </c>
     </row>
@@ -2361,19 +2875,19 @@
       <c r="M22">
         <v>1.3390500000000001</v>
       </c>
-      <c r="N22" s="1">
+      <c r="N22" s="7">
         <v>1.4339999999999999</v>
       </c>
-      <c r="O22" s="1">
+      <c r="O22" s="7">
         <v>1.4339999999999999</v>
       </c>
-      <c r="P22" s="1">
+      <c r="P22" s="7">
         <v>1.4319999999999999</v>
       </c>
-      <c r="Q22" s="1">
+      <c r="Q22" s="7">
         <v>1.4379999999999999</v>
       </c>
-      <c r="R22" s="1">
+      <c r="R22" s="7">
         <v>1.4430000000000001</v>
       </c>
     </row>
@@ -2417,19 +2931,19 @@
       <c r="M23">
         <v>1.33579</v>
       </c>
-      <c r="N23" s="1">
+      <c r="N23" s="7">
         <v>1.3009999999999999</v>
       </c>
-      <c r="O23" s="1">
+      <c r="O23" s="7">
         <v>1.3</v>
       </c>
-      <c r="P23" s="1">
+      <c r="P23" s="7">
         <v>1.3009999999999999</v>
       </c>
-      <c r="Q23" s="1">
+      <c r="Q23" s="7">
         <v>1.3100000000000001</v>
       </c>
-      <c r="R23" s="1">
+      <c r="R23" s="7">
         <v>1.3109999999999999</v>
       </c>
     </row>
@@ -2473,19 +2987,19 @@
       <c r="M24">
         <v>1.3343400000000001</v>
       </c>
-      <c r="N24" s="1">
+      <c r="N24" s="7">
         <v>1.234</v>
       </c>
-      <c r="O24" s="1">
+      <c r="O24" s="7">
         <v>1.232</v>
       </c>
-      <c r="P24" s="1">
+      <c r="P24" s="7">
         <v>1.2330000000000001</v>
       </c>
-      <c r="Q24" s="1">
+      <c r="Q24" s="7">
         <v>1.24</v>
       </c>
-      <c r="R24" s="1">
+      <c r="R24" s="7">
         <v>1.2430000000000001</v>
       </c>
     </row>
@@ -2529,19 +3043,19 @@
       <c r="M25">
         <v>1.3335399999999999</v>
       </c>
-      <c r="N25" s="1">
+      <c r="N25" s="7">
         <v>1.1899999999999999</v>
       </c>
-      <c r="O25" s="1">
+      <c r="O25" s="7">
         <v>1.1879999999999999</v>
       </c>
-      <c r="P25" s="1">
+      <c r="P25" s="7">
         <v>1.1879999999999999</v>
       </c>
-      <c r="Q25" s="1">
+      <c r="Q25" s="7">
         <v>1.194</v>
       </c>
-      <c r="R25" s="1">
+      <c r="R25" s="7">
         <v>1.1990000000000001</v>
       </c>
     </row>
@@ -2564,16 +3078,16 @@
       <c r="N26">
         <v>1.2</v>
       </c>
-      <c r="O26" s="1">
+      <c r="O26" s="7">
         <v>1.1970000000000001</v>
       </c>
-      <c r="P26" s="1">
+      <c r="P26" s="7">
         <v>1.1970000000000001</v>
       </c>
-      <c r="Q26" s="1">
+      <c r="Q26" s="7">
         <v>1.204</v>
       </c>
-      <c r="R26" s="1">
+      <c r="R26" s="7">
         <v>1.208</v>
       </c>
     </row>
@@ -2617,19 +3131,19 @@
       <c r="M27">
         <v>1.3481399999999999</v>
       </c>
-      <c r="N27" s="1">
+      <c r="N27" s="7">
         <v>2.0710000000000002</v>
       </c>
-      <c r="O27" s="1">
+      <c r="O27" s="7">
         <v>2.0699999999999998</v>
       </c>
-      <c r="P27" s="1">
+      <c r="P27" s="7">
         <v>2.0680000000000001</v>
       </c>
-      <c r="Q27" s="1">
+      <c r="Q27" s="7">
         <v>2.077</v>
       </c>
-      <c r="R27" s="1">
+      <c r="R27" s="7">
         <v>2.0830000000000002</v>
       </c>
     </row>
@@ -2673,19 +3187,19 @@
       <c r="M28">
         <v>1.3486899999999999</v>
       </c>
-      <c r="N28" s="1">
+      <c r="N28" s="7">
         <v>2.1459999999999999</v>
       </c>
-      <c r="O28" s="1">
+      <c r="O28" s="7">
         <v>2.1440000000000001</v>
       </c>
-      <c r="P28" s="1">
+      <c r="P28" s="7">
         <v>2.1419999999999999</v>
       </c>
-      <c r="Q28" s="1">
+      <c r="Q28" s="7">
         <v>2.149</v>
       </c>
-      <c r="R28" s="1">
+      <c r="R28" s="7">
         <v>2.1560000000000001</v>
       </c>
     </row>
@@ -2729,19 +3243,19 @@
       <c r="M29">
         <v>1.34839</v>
       </c>
-      <c r="N29" s="1">
+      <c r="N29" s="7">
         <v>2.1520000000000001</v>
       </c>
-      <c r="O29" s="1">
+      <c r="O29" s="7">
         <v>2.1469999999999998</v>
       </c>
-      <c r="P29" s="1">
+      <c r="P29" s="7">
         <v>2.1469999999999998</v>
       </c>
-      <c r="Q29" s="1">
+      <c r="Q29" s="7">
         <v>2.1539999999999999</v>
       </c>
-      <c r="R29" s="1">
+      <c r="R29" s="7">
         <v>2.161</v>
       </c>
     </row>
@@ -2785,19 +3299,19 @@
       <c r="M30">
         <v>1.3484799999999999</v>
       </c>
-      <c r="N30" s="1">
+      <c r="N30" s="7">
         <v>2.0819999999999999</v>
       </c>
-      <c r="O30" s="1">
+      <c r="O30" s="7">
         <v>2.081</v>
       </c>
-      <c r="P30" s="1">
+      <c r="P30" s="7">
         <v>2.0800000000000001</v>
       </c>
-      <c r="Q30" s="1">
+      <c r="Q30" s="7">
         <v>2.0859999999999999</v>
       </c>
-      <c r="R30" s="1">
+      <c r="R30" s="7">
         <v>2.0920000000000001</v>
       </c>
     </row>
@@ -2841,19 +3355,19 @@
       <c r="M31">
         <v>1.34639</v>
       </c>
-      <c r="N31" s="1">
+      <c r="N31" s="7">
         <v>1.716</v>
       </c>
-      <c r="O31" s="1">
+      <c r="O31" s="7">
         <v>1.7150000000000001</v>
       </c>
-      <c r="P31" s="1">
+      <c r="P31" s="7">
         <v>1.7130000000000001</v>
       </c>
-      <c r="Q31" s="1">
+      <c r="Q31" s="7">
         <v>1.7210000000000001</v>
       </c>
-      <c r="R31" s="1">
+      <c r="R31" s="7">
         <v>1.726</v>
       </c>
     </row>
@@ -2897,19 +3411,19 @@
       <c r="M32">
         <v>1.3398699999999999</v>
       </c>
-      <c r="N32" s="1">
+      <c r="N32" s="7">
         <v>1.474</v>
       </c>
-      <c r="O32" s="1">
+      <c r="O32" s="7">
         <v>1.472</v>
       </c>
-      <c r="P32" s="1">
+      <c r="P32" s="7">
         <v>1.472</v>
       </c>
-      <c r="Q32" s="1">
+      <c r="Q32" s="7">
         <v>1.4790000000000001</v>
       </c>
-      <c r="R32" s="1">
+      <c r="R32" s="7">
         <v>1.482</v>
       </c>
     </row>
@@ -2953,19 +3467,19 @@
       <c r="M33">
         <v>1.3366899999999999</v>
       </c>
-      <c r="N33" s="1">
+      <c r="N33" s="7">
         <v>1.355</v>
       </c>
-      <c r="O33" s="1">
+      <c r="O33" s="7">
         <v>1.353</v>
       </c>
-      <c r="P33" s="1">
+      <c r="P33" s="7">
         <v>1.3540000000000001</v>
       </c>
-      <c r="Q33" s="1">
+      <c r="Q33" s="7">
         <v>1.361</v>
       </c>
-      <c r="R33" s="1">
+      <c r="R33" s="7">
         <v>1.365</v>
       </c>
     </row>
@@ -3009,19 +3523,19 @@
       <c r="M34">
         <v>1.3348100000000001</v>
       </c>
-      <c r="N34" s="1">
+      <c r="N34" s="7">
         <v>1.26</v>
       </c>
-      <c r="O34" s="1">
+      <c r="O34" s="7">
         <v>1.256</v>
       </c>
-      <c r="P34" s="1">
+      <c r="P34" s="7">
         <v>1.2569999999999999</v>
       </c>
-      <c r="Q34" s="1">
+      <c r="Q34" s="7">
         <v>1.266</v>
       </c>
-      <c r="R34" s="1">
+      <c r="R34" s="7">
         <v>1.2689999999999999</v>
       </c>
     </row>
@@ -3065,19 +3579,19 @@
       <c r="M35">
         <v>1.33395</v>
       </c>
-      <c r="N35" s="1">
+      <c r="N35" s="7">
         <v>1.2230000000000001</v>
       </c>
-      <c r="O35" s="1">
+      <c r="O35" s="7">
         <v>1.2210000000000001</v>
       </c>
-      <c r="P35" s="1">
+      <c r="P35" s="7">
         <v>1.22</v>
       </c>
-      <c r="Q35" s="1">
+      <c r="Q35" s="7">
         <v>1.228</v>
       </c>
-      <c r="R35" s="1">
+      <c r="R35" s="7">
         <v>1.2310000000000001</v>
       </c>
     </row>
@@ -3121,19 +3635,19 @@
       <c r="M36">
         <v>1.34605</v>
       </c>
-      <c r="N36" s="1">
+      <c r="N36" s="7">
         <v>1.653</v>
       </c>
-      <c r="O36" s="1">
+      <c r="O36" s="7">
         <v>1.6499999999999999</v>
       </c>
-      <c r="P36" s="1">
+      <c r="P36" s="7">
         <v>1.6499999999999999</v>
       </c>
-      <c r="Q36" s="1">
+      <c r="Q36" s="7">
         <v>1.6559999999999999</v>
       </c>
-      <c r="R36" s="1">
+      <c r="R36" s="7">
         <v>1.6599999999999999</v>
       </c>
     </row>
@@ -3177,19 +3691,19 @@
       <c r="M37">
         <v>1.33874</v>
       </c>
-      <c r="N37" s="1">
+      <c r="N37" s="7">
         <v>1.405</v>
       </c>
-      <c r="O37" s="1">
+      <c r="O37" s="7">
         <v>1.4039999999999999</v>
       </c>
-      <c r="P37" s="1">
+      <c r="P37" s="7">
         <v>1.403</v>
       </c>
-      <c r="Q37" s="1">
+      <c r="Q37" s="7">
         <v>1.4099999999999999</v>
       </c>
-      <c r="R37" s="1">
+      <c r="R37" s="7">
         <v>1.413</v>
       </c>
     </row>
@@ -3233,19 +3747,19 @@
       <c r="M38">
         <v>1.33578</v>
       </c>
-      <c r="N38" s="1">
+      <c r="N38" s="7">
         <v>1.272</v>
       </c>
       <c r="O38">
         <v>1.268</v>
       </c>
-      <c r="P38" s="1">
+      <c r="P38" s="7">
         <v>1.2689999999999999</v>
       </c>
-      <c r="Q38" s="1">
+      <c r="Q38" s="7">
         <v>1.276</v>
       </c>
-      <c r="R38" s="1">
+      <c r="R38" s="7">
         <v>1.2789999999999999</v>
       </c>
     </row>
@@ -3289,19 +3803,19 @@
       <c r="M39">
         <v>1.3344800000000001</v>
       </c>
-      <c r="N39" s="1">
+      <c r="N39" s="7">
         <v>1.232</v>
       </c>
-      <c r="O39" s="1">
+      <c r="O39" s="7">
         <v>1.2310000000000001</v>
       </c>
-      <c r="P39" s="1">
+      <c r="P39" s="7">
         <v>1.2310000000000001</v>
       </c>
-      <c r="Q39" s="1">
+      <c r="Q39" s="7">
         <v>1.2370000000000001</v>
       </c>
-      <c r="R39" s="1">
+      <c r="R39" s="7">
         <v>1.24</v>
       </c>
     </row>
@@ -3345,19 +3859,19 @@
       <c r="M40">
         <v>1.33368</v>
       </c>
-      <c r="N40" s="1">
+      <c r="N40" s="7">
         <v>1.1930000000000001</v>
       </c>
-      <c r="O40" s="1">
+      <c r="O40" s="7">
         <v>1.1879999999999999</v>
       </c>
-      <c r="P40" s="1">
+      <c r="P40" s="7">
         <v>1.1899999999999999</v>
       </c>
-      <c r="Q40" s="1">
+      <c r="Q40" s="7">
         <v>1.1970000000000001</v>
       </c>
-      <c r="R40" s="1">
+      <c r="R40" s="7">
         <v>1.1990000000000001</v>
       </c>
     </row>
@@ -3401,19 +3915,19 @@
       <c r="M41">
         <v>1.3468500000000001</v>
       </c>
-      <c r="N41" s="1">
+      <c r="N41" s="7">
         <v>1.855</v>
       </c>
-      <c r="O41" s="1">
+      <c r="O41" s="7">
         <v>1.853</v>
       </c>
-      <c r="P41" s="1">
+      <c r="P41" s="7">
         <v>1.8540000000000001</v>
       </c>
-      <c r="Q41" s="1">
+      <c r="Q41" s="7">
         <v>1.859</v>
       </c>
-      <c r="R41" s="1">
+      <c r="R41" s="7">
         <v>1.863</v>
       </c>
     </row>
@@ -3457,19 +3971,19 @@
       <c r="M42">
         <v>1.3392299999999999</v>
       </c>
-      <c r="N42" s="1">
+      <c r="N42" s="7">
         <v>1.4850000000000001</v>
       </c>
-      <c r="O42" s="1">
+      <c r="O42" s="7">
         <v>1.482</v>
       </c>
-      <c r="P42" s="1">
+      <c r="P42" s="7">
         <v>1.484</v>
       </c>
-      <c r="Q42" s="1">
+      <c r="Q42" s="7">
         <v>1.49</v>
       </c>
-      <c r="R42" s="1">
+      <c r="R42" s="7">
         <v>1.4930000000000001</v>
       </c>
     </row>
@@ -3513,19 +4027,19 @@
       <c r="M43">
         <v>1.3359300000000001</v>
       </c>
-      <c r="N43" s="1">
+      <c r="N43" s="7">
         <v>1.3080000000000001</v>
       </c>
-      <c r="O43" s="1">
+      <c r="O43" s="7">
         <v>1.306</v>
       </c>
-      <c r="P43" s="1">
+      <c r="P43" s="7">
         <v>1.3049999999999999</v>
       </c>
-      <c r="Q43" s="1">
+      <c r="Q43" s="7">
         <v>1.3140000000000001</v>
       </c>
-      <c r="R43" s="1">
+      <c r="R43" s="7">
         <v>1.3149999999999999</v>
       </c>
     </row>
@@ -3569,19 +4083,19 @@
       <c r="M44">
         <v>1.3344199999999999</v>
       </c>
-      <c r="N44" s="1">
+      <c r="N44" s="7">
         <v>1.2689999999999999</v>
       </c>
-      <c r="O44" s="1">
+      <c r="O44" s="7">
         <v>1.2669999999999999</v>
       </c>
-      <c r="P44" s="1">
+      <c r="P44" s="7">
         <v>1.2649999999999999</v>
       </c>
-      <c r="Q44" s="1">
+      <c r="Q44" s="7">
         <v>1.272</v>
       </c>
-      <c r="R44" s="1">
+      <c r="R44" s="7">
         <v>1.276</v>
       </c>
     </row>
@@ -3625,19 +4139,19 @@
       <c r="M45">
         <v>1.3337000000000001</v>
       </c>
-      <c r="N45" s="1">
+      <c r="N45" s="7">
         <v>1.224</v>
       </c>
-      <c r="O45" s="1">
+      <c r="O45" s="7">
         <v>1.222</v>
       </c>
-      <c r="P45" s="1">
+      <c r="P45" s="7">
         <v>1.222</v>
       </c>
-      <c r="Q45" s="1">
+      <c r="Q45" s="7">
         <v>1.228</v>
       </c>
-      <c r="R45" s="1">
+      <c r="R45" s="7">
         <v>1.23</v>
       </c>
     </row>
@@ -3681,19 +4195,19 @@
       <c r="M46">
         <v>1.3470299999999999</v>
       </c>
-      <c r="N46" s="1">
+      <c r="N46" s="7">
         <v>1.784</v>
       </c>
-      <c r="O46" s="1">
+      <c r="O46" s="7">
         <v>1.7829999999999999</v>
       </c>
-      <c r="P46" s="1">
+      <c r="P46" s="7">
         <v>1.7829999999999999</v>
       </c>
-      <c r="Q46" s="1">
+      <c r="Q46" s="7">
         <v>1.788</v>
       </c>
-      <c r="R46" s="1">
+      <c r="R46" s="7">
         <v>1.792</v>
       </c>
     </row>
@@ -3713,7 +4227,7 @@
       <c r="E47">
         <v>0</v>
       </c>
-      <c r="F47" s="2">
+      <c r="F47" s="4">
         <v>18</v>
       </c>
       <c r="G47">
@@ -3737,19 +4251,19 @@
       <c r="M47">
         <v>1.33985</v>
       </c>
-      <c r="N47" s="1">
+      <c r="N47" s="7">
         <v>1.508</v>
       </c>
-      <c r="O47" s="1">
+      <c r="O47" s="7">
         <v>1.5069999999999999</v>
       </c>
-      <c r="P47" s="1">
+      <c r="P47" s="7">
         <v>1.506</v>
       </c>
-      <c r="Q47" s="1">
+      <c r="Q47" s="7">
         <v>1.5109999999999999</v>
       </c>
-      <c r="R47" s="1">
+      <c r="R47" s="7">
         <v>1.516</v>
       </c>
     </row>
@@ -3784,7 +4298,7 @@
       <c r="J48">
         <v>1.77</v>
       </c>
-      <c r="K48" s="1">
+      <c r="K48" s="7">
         <v>1.8400000000000001</v>
       </c>
       <c r="L48">
@@ -3793,19 +4307,19 @@
       <c r="M48">
         <v>1.3362400000000001</v>
       </c>
-      <c r="N48" s="1">
+      <c r="N48" s="7">
         <v>1.3520000000000001</v>
       </c>
-      <c r="O48" s="1">
+      <c r="O48" s="7">
         <v>1.351</v>
       </c>
-      <c r="P48" s="1">
+      <c r="P48" s="7">
         <v>1.351</v>
       </c>
-      <c r="Q48" s="1">
+      <c r="Q48" s="7">
         <v>1.357</v>
       </c>
-      <c r="R48" s="1">
+      <c r="R48" s="7">
         <v>1.361</v>
       </c>
     </row>
@@ -3849,19 +4363,19 @@
       <c r="M49">
         <v>1.3346499999999999</v>
       </c>
-      <c r="N49" s="1">
+      <c r="N49" s="7">
         <v>1.258</v>
       </c>
-      <c r="O49" s="1">
+      <c r="O49" s="7">
         <v>1.2569999999999999</v>
       </c>
-      <c r="P49" s="1">
+      <c r="P49" s="7">
         <v>1.2569999999999999</v>
       </c>
-      <c r="Q49" s="1">
+      <c r="Q49" s="7">
         <v>1.2629999999999999</v>
       </c>
-      <c r="R49" s="1">
+      <c r="R49" s="7">
         <v>1.266</v>
       </c>
     </row>
@@ -3905,19 +4419,19 @@
       <c r="M50">
         <v>1.3338000000000001</v>
       </c>
-      <c r="N50" s="1">
+      <c r="N50" s="7">
         <v>1.2210000000000001</v>
       </c>
-      <c r="O50" s="1">
+      <c r="O50" s="7">
         <v>1.22</v>
       </c>
-      <c r="P50" s="1">
+      <c r="P50" s="7">
         <v>1.2190000000000001</v>
       </c>
-      <c r="Q50" s="1">
+      <c r="Q50" s="7">
         <v>1.2250000000000001</v>
       </c>
-      <c r="R50" s="1">
+      <c r="R50" s="7">
         <v>1.228</v>
       </c>
     </row>
@@ -3934,30 +4448,30 @@
       <c r="H51">
         <v>1.1910000000000001</v>
       </c>
-      <c r="I51" s="2">
+      <c r="I51" s="4">
         <v>1.1910000000000001</v>
       </c>
       <c r="N51">
         <v>1.1930000000000001</v>
       </c>
-      <c r="O51" s="1">
+      <c r="O51" s="7">
         <v>1.1899999999999999</v>
       </c>
-      <c r="P51" s="1">
+      <c r="P51" s="7">
         <v>1.1899999999999999</v>
       </c>
-      <c r="Q51" s="1">
+      <c r="Q51" s="7">
         <v>1.196</v>
       </c>
-      <c r="R51" s="1">
+      <c r="R51" s="7">
         <v>1.198</v>
       </c>
     </row>
     <row r="52" ht="14.25">
-      <c r="A52" s="2">
+      <c r="A52" s="4">
         <v>51</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52" s="4">
         <v>18</v>
       </c>
       <c r="C52">
@@ -3975,7 +4489,7 @@
       <c r="G52">
         <v>1.3329899999999999</v>
       </c>
-      <c r="H52" s="1">
+      <c r="H52" s="7">
         <v>1.1830000000000001</v>
       </c>
       <c r="I52">
@@ -3993,27 +4507,27 @@
       <c r="M52">
         <v>1.3482499999999999</v>
       </c>
-      <c r="N52" s="1">
+      <c r="N52" s="7">
         <v>2.0019999999999998</v>
       </c>
-      <c r="O52" s="1">
+      <c r="O52" s="7">
         <v>2.0009999999999999</v>
       </c>
-      <c r="P52" s="1">
+      <c r="P52" s="7">
         <v>2.0009999999999999</v>
       </c>
-      <c r="Q52" s="1">
+      <c r="Q52" s="7">
         <v>2.0070000000000001</v>
       </c>
-      <c r="R52" s="1">
+      <c r="R52" s="7">
         <v>2.0139999999999998</v>
       </c>
     </row>
     <row r="53" ht="14.25">
-      <c r="A53" s="2">
+      <c r="A53" s="4">
         <v>52</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="4">
         <v>19</v>
       </c>
       <c r="C53">
@@ -4049,27 +4563,27 @@
       <c r="M53">
         <v>1.3487100000000001</v>
       </c>
-      <c r="N53" s="1">
+      <c r="N53" s="7">
         <v>1.966</v>
       </c>
-      <c r="O53" s="1">
+      <c r="O53" s="7">
         <v>1.9650000000000001</v>
       </c>
-      <c r="P53" s="1">
+      <c r="P53" s="7">
         <v>1.962</v>
       </c>
-      <c r="Q53" s="1">
+      <c r="Q53" s="7">
         <v>1.97</v>
       </c>
-      <c r="R53" s="1">
+      <c r="R53" s="7">
         <v>1.976</v>
       </c>
     </row>
     <row r="54" ht="14.25">
-      <c r="A54" s="2">
+      <c r="A54" s="4">
         <v>53</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54" s="4">
         <v>20</v>
       </c>
       <c r="C54">
@@ -4105,27 +4619,27 @@
       <c r="M54">
         <v>1.3486499999999999</v>
       </c>
-      <c r="N54" s="1">
+      <c r="N54" s="7">
         <v>2.0369999999999999</v>
       </c>
-      <c r="O54" s="1">
+      <c r="O54" s="7">
         <v>2.036</v>
       </c>
-      <c r="P54" s="1">
+      <c r="P54" s="7">
         <v>2.0339999999999998</v>
       </c>
-      <c r="Q54" s="1">
+      <c r="Q54" s="7">
         <v>2.0409999999999999</v>
       </c>
-      <c r="R54" s="1">
+      <c r="R54" s="7">
         <v>2.048</v>
       </c>
     </row>
     <row r="55" ht="14.25">
-      <c r="A55" s="2">
+      <c r="A55" s="4">
         <v>54</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55" s="4">
         <v>21</v>
       </c>
       <c r="C55">
@@ -4161,27 +4675,27 @@
       <c r="M55">
         <v>1.3495299999999999</v>
       </c>
-      <c r="N55" s="1">
+      <c r="N55" s="7">
         <v>2.0299999999999998</v>
       </c>
-      <c r="O55" s="1">
+      <c r="O55" s="7">
         <v>2.028</v>
       </c>
-      <c r="P55" s="1">
+      <c r="P55" s="7">
         <v>2.0270000000000001</v>
       </c>
-      <c r="Q55" s="1">
+      <c r="Q55" s="7">
         <v>2.0329999999999999</v>
       </c>
-      <c r="R55" s="1">
+      <c r="R55" s="7">
         <v>2.0409999999999999</v>
       </c>
     </row>
     <row r="56" ht="14.25">
-      <c r="A56" s="2">
+      <c r="A56" s="4">
         <v>55</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B56" s="4">
         <v>22</v>
       </c>
       <c r="C56">
@@ -4217,27 +4731,27 @@
       <c r="M56">
         <v>1.3468</v>
       </c>
-      <c r="N56" s="1">
+      <c r="N56" s="7">
         <v>1.895</v>
       </c>
-      <c r="O56" s="1">
+      <c r="O56" s="7">
         <v>1.8939999999999999</v>
       </c>
-      <c r="P56" s="1">
+      <c r="P56" s="7">
         <v>1.893</v>
       </c>
-      <c r="Q56" s="1">
+      <c r="Q56" s="7">
         <v>1.8999999999999999</v>
       </c>
-      <c r="R56" s="1">
+      <c r="R56" s="7">
         <v>1.907</v>
       </c>
     </row>
     <row r="57" ht="14.25">
-      <c r="A57" s="2">
+      <c r="A57" s="4">
         <v>56</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B57" s="4">
         <v>22</v>
       </c>
       <c r="C57">
@@ -4273,27 +4787,27 @@
       <c r="M57">
         <v>1.3397399999999999</v>
       </c>
-      <c r="N57" s="1">
+      <c r="N57" s="7">
         <v>1.548</v>
       </c>
-      <c r="O57" s="1">
+      <c r="O57" s="7">
         <v>1.548</v>
       </c>
-      <c r="P57" s="1">
+      <c r="P57" s="7">
         <v>1.548</v>
       </c>
-      <c r="Q57" s="1">
+      <c r="Q57" s="7">
         <v>1.5549999999999999</v>
       </c>
-      <c r="R57" s="1">
+      <c r="R57" s="7">
         <v>1.5609999999999999</v>
       </c>
     </row>
     <row r="58" ht="14.25">
-      <c r="A58" s="2">
+      <c r="A58" s="4">
         <v>57</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="4">
         <v>22</v>
       </c>
       <c r="C58">
@@ -4329,27 +4843,27 @@
       <c r="M58">
         <v>1.3362400000000001</v>
       </c>
-      <c r="N58" s="1">
+      <c r="N58" s="7">
         <v>1.363</v>
       </c>
-      <c r="O58" s="1">
+      <c r="O58" s="7">
         <v>1.359</v>
       </c>
-      <c r="P58" s="1">
+      <c r="P58" s="7">
         <v>1.3580000000000001</v>
       </c>
-      <c r="Q58" s="1">
+      <c r="Q58" s="7">
         <v>1.367</v>
       </c>
-      <c r="R58" s="1">
+      <c r="R58" s="7">
         <v>1.3720000000000001</v>
       </c>
     </row>
     <row r="59" ht="14.25">
-      <c r="A59" s="2">
+      <c r="A59" s="4">
         <v>58</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B59" s="4">
         <v>22</v>
       </c>
       <c r="C59">
@@ -4385,27 +4899,27 @@
       <c r="M59">
         <v>1.33467</v>
       </c>
-      <c r="N59" s="1">
+      <c r="N59" s="7">
         <v>1.276</v>
       </c>
-      <c r="O59" s="1">
+      <c r="O59" s="7">
         <v>1.272</v>
       </c>
-      <c r="P59" s="1">
+      <c r="P59" s="7">
         <v>1.272</v>
       </c>
-      <c r="Q59" s="1">
+      <c r="Q59" s="7">
         <v>1.282</v>
       </c>
-      <c r="R59" s="1">
+      <c r="R59" s="7">
         <v>1.2849999999999999</v>
       </c>
     </row>
     <row r="60" ht="14.25">
-      <c r="A60" s="2">
+      <c r="A60" s="4">
         <v>59</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B60" s="4">
         <v>22</v>
       </c>
       <c r="C60">
@@ -4441,27 +4955,27 @@
       <c r="M60">
         <v>1.3338099999999999</v>
       </c>
-      <c r="N60" s="1">
+      <c r="N60" s="7">
         <v>1.2390000000000001</v>
       </c>
-      <c r="O60" s="1">
+      <c r="O60" s="7">
         <v>1.236</v>
       </c>
-      <c r="P60" s="1">
+      <c r="P60" s="7">
         <v>1.236</v>
       </c>
-      <c r="Q60" s="1">
+      <c r="Q60" s="7">
         <v>1.2450000000000001</v>
       </c>
-      <c r="R60" s="1">
+      <c r="R60" s="7">
         <v>1.2490000000000001</v>
       </c>
     </row>
     <row r="61" ht="14.25">
-      <c r="A61" s="2">
+      <c r="A61" s="4">
         <v>60</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B61" s="4">
         <v>23</v>
       </c>
       <c r="C61">
@@ -4497,27 +5011,27 @@
       <c r="M61">
         <v>1.3475200000000001</v>
       </c>
-      <c r="N61" s="1">
+      <c r="N61" s="7">
         <v>1.946</v>
       </c>
-      <c r="O61" s="1">
+      <c r="O61" s="7">
         <v>1.9419999999999999</v>
       </c>
-      <c r="P61" s="1">
+      <c r="P61" s="7">
         <v>1.9419999999999999</v>
       </c>
-      <c r="Q61" s="1">
+      <c r="Q61" s="7">
         <v>1.9510000000000001</v>
       </c>
-      <c r="R61" s="1">
+      <c r="R61" s="7">
         <v>1.954</v>
       </c>
     </row>
     <row r="62" ht="14.25">
-      <c r="A62" s="2">
+      <c r="A62" s="4">
         <v>61</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62" s="4">
         <v>23</v>
       </c>
       <c r="C62">
@@ -4553,27 +5067,27 @@
       <c r="M62">
         <v>1.3396699999999999</v>
       </c>
-      <c r="N62" s="1">
+      <c r="N62" s="7">
         <v>1.528</v>
       </c>
-      <c r="O62" s="1">
+      <c r="O62" s="7">
         <v>1.5229999999999999</v>
       </c>
-      <c r="P62" s="1">
+      <c r="P62" s="7">
         <v>1.5229999999999999</v>
       </c>
-      <c r="Q62" s="1">
+      <c r="Q62" s="7">
         <v>1.5329999999999999</v>
       </c>
-      <c r="R62" s="1">
+      <c r="R62" s="7">
         <v>1.5369999999999999</v>
       </c>
     </row>
     <row r="63" ht="14.25">
-      <c r="A63" s="2">
+      <c r="A63" s="4">
         <v>62</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63" s="4">
         <v>23</v>
       </c>
       <c r="C63">
@@ -4609,27 +5123,27 @@
       <c r="M63">
         <v>1.33596</v>
       </c>
-      <c r="N63" s="1">
+      <c r="N63" s="7">
         <v>1.29</v>
       </c>
-      <c r="O63" s="1">
+      <c r="O63" s="7">
         <v>1.2849999999999999</v>
       </c>
-      <c r="P63" s="1">
+      <c r="P63" s="7">
         <v>1.284</v>
       </c>
-      <c r="Q63" s="1">
+      <c r="Q63" s="7">
         <v>1.294</v>
       </c>
-      <c r="R63" s="1">
+      <c r="R63" s="7">
         <v>1.298</v>
       </c>
     </row>
     <row r="64" ht="14.25">
-      <c r="A64" s="2">
+      <c r="A64" s="4">
         <v>63</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64" s="4">
         <v>23</v>
       </c>
       <c r="C64">
@@ -4665,27 +5179,27 @@
       <c r="M64">
         <v>1.3344</v>
       </c>
-      <c r="N64" s="1">
+      <c r="N64" s="7">
         <v>1.2789999999999999</v>
       </c>
-      <c r="O64" s="1">
+      <c r="O64" s="7">
         <v>1.2749999999999999</v>
       </c>
-      <c r="P64" s="1">
+      <c r="P64" s="7">
         <v>1.2749999999999999</v>
       </c>
-      <c r="Q64" s="1">
+      <c r="Q64" s="7">
         <v>1.284</v>
       </c>
-      <c r="R64" s="1">
+      <c r="R64" s="7">
         <v>1.288</v>
       </c>
     </row>
     <row r="65" ht="14.25">
-      <c r="A65" s="2">
+      <c r="A65" s="4">
         <v>64</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B65" s="4">
         <v>23</v>
       </c>
       <c r="C65">
@@ -4721,27 +5235,27 @@
       <c r="M65">
         <v>1.33368</v>
       </c>
-      <c r="N65" s="1">
+      <c r="N65" s="7">
         <v>1.248</v>
       </c>
-      <c r="O65" s="1">
+      <c r="O65" s="7">
         <v>1.2430000000000001</v>
       </c>
-      <c r="P65" s="1">
+      <c r="P65" s="7">
         <v>1.242</v>
       </c>
-      <c r="Q65" s="1">
+      <c r="Q65" s="7">
         <v>1.2529999999999999</v>
       </c>
-      <c r="R65" s="1">
+      <c r="R65" s="7">
         <v>1.256</v>
       </c>
     </row>
     <row r="66" ht="14.25">
-      <c r="A66" s="2">
+      <c r="A66" s="4">
         <v>65</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B66" s="4">
         <v>24</v>
       </c>
       <c r="C66">
@@ -4777,27 +5291,27 @@
       <c r="M66">
         <v>1.3473999999999999</v>
       </c>
-      <c r="N66" s="1">
+      <c r="N66" s="7">
         <v>1.8380000000000001</v>
       </c>
-      <c r="O66" s="1">
+      <c r="O66" s="7">
         <v>1.8340000000000001</v>
       </c>
-      <c r="P66" s="1">
+      <c r="P66" s="7">
         <v>1.833</v>
       </c>
-      <c r="Q66" s="1">
+      <c r="Q66" s="7">
         <v>1.841</v>
       </c>
-      <c r="R66" s="1">
+      <c r="R66" s="7">
         <v>1.8460000000000001</v>
       </c>
     </row>
     <row r="67" ht="14.25">
-      <c r="A67" s="2">
+      <c r="A67" s="4">
         <v>66</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B67" s="4">
         <v>24</v>
       </c>
       <c r="C67">
@@ -4833,27 +5347,27 @@
       <c r="M67">
         <v>1.3405800000000001</v>
       </c>
-      <c r="N67" s="1">
+      <c r="N67" s="7">
         <v>1.5549999999999999</v>
       </c>
-      <c r="O67" s="1">
+      <c r="O67" s="7">
         <v>1.554</v>
       </c>
-      <c r="P67" s="1">
+      <c r="P67" s="7">
         <v>1.5529999999999999</v>
       </c>
-      <c r="Q67" s="1">
+      <c r="Q67" s="7">
         <v>1.5600000000000001</v>
       </c>
-      <c r="R67" s="1">
+      <c r="R67" s="7">
         <v>1.5649999999999999</v>
       </c>
     </row>
     <row r="68" ht="14.25">
-      <c r="A68" s="2">
+      <c r="A68" s="4">
         <v>67</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B68" s="4">
         <v>24</v>
       </c>
       <c r="C68">
@@ -4889,27 +5403,27 @@
       <c r="M68">
         <v>1.3367899999999999</v>
       </c>
-      <c r="N68" s="1">
+      <c r="N68" s="7">
         <v>1.371</v>
       </c>
-      <c r="O68" s="1">
+      <c r="O68" s="7">
         <v>1.367</v>
       </c>
-      <c r="P68" s="1">
+      <c r="P68" s="7">
         <v>1.367</v>
       </c>
-      <c r="Q68" s="1">
+      <c r="Q68" s="7">
         <v>1.3759999999999999</v>
       </c>
-      <c r="R68" s="1">
+      <c r="R68" s="7">
         <v>1.379</v>
       </c>
     </row>
     <row r="69" ht="14.25">
-      <c r="A69" s="2">
+      <c r="A69" s="4">
         <v>68</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B69" s="4">
         <v>24</v>
       </c>
       <c r="C69">
@@ -4945,27 +5459,27 @@
       <c r="M69">
         <v>1.33494</v>
       </c>
-      <c r="N69" s="1">
+      <c r="N69" s="7">
         <v>1.3069999999999999</v>
       </c>
-      <c r="O69" s="1">
+      <c r="O69" s="7">
         <v>1.304</v>
       </c>
-      <c r="P69" s="1">
+      <c r="P69" s="7">
         <v>1.304</v>
       </c>
-      <c r="Q69" s="1">
+      <c r="Q69" s="7">
         <v>1.3140000000000001</v>
       </c>
-      <c r="R69" s="1">
+      <c r="R69" s="7">
         <v>1.3169999999999999</v>
       </c>
     </row>
     <row r="70" ht="14.25">
-      <c r="A70" s="2">
+      <c r="A70" s="4">
         <v>69</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B70" s="4">
         <v>24</v>
       </c>
       <c r="C70">
@@ -5001,27 +5515,27 @@
       <c r="M70">
         <v>1.33395</v>
       </c>
-      <c r="N70" s="1">
+      <c r="N70" s="7">
         <v>1.216</v>
       </c>
-      <c r="O70" s="1">
+      <c r="O70" s="7">
         <v>1.212</v>
       </c>
-      <c r="P70" s="1">
+      <c r="P70" s="7">
         <v>1.2110000000000001</v>
       </c>
-      <c r="Q70" s="1">
+      <c r="Q70" s="7">
         <v>1.2210000000000001</v>
       </c>
-      <c r="R70" s="1">
+      <c r="R70" s="7">
         <v>1.222</v>
       </c>
     </row>
     <row r="71" ht="14.25">
-      <c r="A71" s="2">
+      <c r="A71" s="4">
         <v>70</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B71" s="4">
         <v>25</v>
       </c>
       <c r="C71">
@@ -5057,27 +5571,27 @@
       <c r="M71">
         <v>1.34826</v>
       </c>
-      <c r="N71" s="1">
+      <c r="N71" s="7">
         <v>1.974</v>
       </c>
-      <c r="O71" s="1">
+      <c r="O71" s="7">
         <v>1.97</v>
       </c>
-      <c r="P71" s="1">
+      <c r="P71" s="7">
         <v>1.968</v>
       </c>
-      <c r="Q71" s="1">
+      <c r="Q71" s="7">
         <v>1.9770000000000001</v>
       </c>
-      <c r="R71" s="1">
+      <c r="R71" s="7">
         <v>1.9790000000000001</v>
       </c>
     </row>
     <row r="72" ht="14.25">
-      <c r="A72" s="2">
+      <c r="A72" s="4">
         <v>71</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B72" s="4">
         <v>25</v>
       </c>
       <c r="C72">
@@ -5113,27 +5627,27 @@
       <c r="M72">
         <v>1.33989</v>
       </c>
-      <c r="N72" s="1">
+      <c r="N72" s="7">
         <v>1.53</v>
       </c>
-      <c r="O72" s="1">
+      <c r="O72" s="7">
         <v>1.528</v>
       </c>
-      <c r="P72" s="1">
+      <c r="P72" s="7">
         <v>1.528</v>
       </c>
-      <c r="Q72" s="1">
+      <c r="Q72" s="7">
         <v>1.5369999999999999</v>
       </c>
-      <c r="R72" s="1">
+      <c r="R72" s="7">
         <v>1.5389999999999999</v>
       </c>
     </row>
     <row r="73" ht="14.25">
-      <c r="A73" s="2">
+      <c r="A73" s="4">
         <v>72</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B73" s="4">
         <v>25</v>
       </c>
       <c r="C73">
@@ -5169,27 +5683,27 @@
       <c r="M73">
         <v>1.3360799999999999</v>
       </c>
-      <c r="N73" s="1">
+      <c r="N73" s="7">
         <v>1.2969999999999999</v>
       </c>
-      <c r="O73" s="1">
+      <c r="O73" s="7">
         <v>1.296</v>
       </c>
-      <c r="P73" s="1">
+      <c r="P73" s="7">
         <v>1.2949999999999999</v>
       </c>
-      <c r="Q73" s="1">
+      <c r="Q73" s="7">
         <v>1.304</v>
       </c>
-      <c r="R73" s="1">
+      <c r="R73" s="7">
         <v>1.3049999999999999</v>
       </c>
     </row>
     <row r="74" ht="14.25">
-      <c r="A74" s="2">
+      <c r="A74" s="4">
         <v>73</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B74" s="4">
         <v>25</v>
       </c>
       <c r="C74">
@@ -5225,27 +5739,27 @@
       <c r="M74">
         <v>1.3345800000000001</v>
       </c>
-      <c r="N74" s="1">
+      <c r="N74" s="7">
         <v>1.3100000000000001</v>
       </c>
-      <c r="O74" s="1">
+      <c r="O74" s="7">
         <v>1.3069999999999999</v>
       </c>
-      <c r="P74" s="1">
+      <c r="P74" s="7">
         <v>1.306</v>
       </c>
-      <c r="Q74" s="1">
+      <c r="Q74" s="7">
         <v>1.3160000000000001</v>
       </c>
-      <c r="R74" s="1">
+      <c r="R74" s="7">
         <v>1.3180000000000001</v>
       </c>
     </row>
     <row r="75" ht="14.25">
-      <c r="A75" s="2">
+      <c r="A75" s="4">
         <v>74</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B75" s="4">
         <v>25</v>
       </c>
       <c r="C75">
@@ -5281,27 +5795,27 @@
       <c r="M75">
         <v>1.33371</v>
       </c>
-      <c r="N75" s="1">
+      <c r="N75" s="7">
         <v>1.2470000000000001</v>
       </c>
-      <c r="O75" s="1">
+      <c r="O75" s="7">
         <v>1.2430000000000001</v>
       </c>
-      <c r="P75" s="1">
+      <c r="P75" s="7">
         <v>1.2430000000000001</v>
       </c>
-      <c r="Q75" s="1">
+      <c r="Q75" s="7">
         <v>1.252</v>
       </c>
-      <c r="R75" s="1">
+      <c r="R75" s="7">
         <v>1.2529999999999999</v>
       </c>
     </row>
     <row r="76" ht="14.25">
-      <c r="A76" s="2">
+      <c r="A76" s="4">
         <v>75</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B76" s="4">
         <v>9</v>
       </c>
       <c r="C76">
@@ -5316,383 +5830,383 @@
       <c r="N76">
         <v>1.1859999999999999</v>
       </c>
-      <c r="O76" s="1">
+      <c r="O76" s="7">
         <v>1.1850000000000001</v>
       </c>
-      <c r="P76" s="1">
+      <c r="P76" s="7">
         <v>1.1839999999999999</v>
       </c>
-      <c r="Q76" s="1">
+      <c r="Q76" s="7">
         <v>1.1910000000000001</v>
       </c>
-      <c r="R76" s="1">
+      <c r="R76" s="7">
         <v>1.1919999999999999</v>
       </c>
     </row>
     <row r="77" ht="14.25">
-      <c r="A77" s="2"/>
-      <c r="B77" s="2"/>
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
     </row>
     <row r="78" ht="14.25">
-      <c r="A78" s="2"/>
-      <c r="B78" s="2"/>
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
     </row>
     <row r="79" ht="14.25">
-      <c r="A79" s="2"/>
-      <c r="B79" s="2"/>
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
     </row>
     <row r="80" ht="14.25">
-      <c r="A80" s="2"/>
-      <c r="B80" s="2"/>
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
     </row>
     <row r="81" ht="14.25">
-      <c r="A81" s="2"/>
-      <c r="B81" s="2"/>
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
     </row>
     <row r="82" ht="14.25">
-      <c r="A82" s="2"/>
-      <c r="B82" s="2"/>
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
     </row>
     <row r="83" ht="14.25">
-      <c r="A83" s="2"/>
-      <c r="B83" s="2"/>
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
     </row>
     <row r="84" ht="14.25">
-      <c r="A84" s="2"/>
-      <c r="B84" s="2"/>
+      <c r="A84" s="4"/>
+      <c r="B84" s="4"/>
     </row>
     <row r="85" ht="14.25">
-      <c r="A85" s="2"/>
-      <c r="B85" s="2"/>
+      <c r="A85" s="4"/>
+      <c r="B85" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="E1" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="4">
+      <c r="A2" s="8">
         <v>44900</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="9">
         <v>0.55208333333333337</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="9">
         <v>0.625</v>
       </c>
-      <c r="D2" s="3">
-        <f>(C2-B2)*24</f>
+      <c r="D2" s="1">
+        <f t="shared" ref="D2:D9" si="0">(C2-B2)*24</f>
         <v>1.7499999999999991</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3">
-      <c r="A3" s="4">
+      <c r="A3" s="8">
         <v>44900</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="9">
         <v>0.625</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="9">
         <v>0.67361111111111116</v>
       </c>
-      <c r="D3" s="3">
-        <f>(C3-B3)*24</f>
+      <c r="D3" s="1">
+        <f t="shared" si="0"/>
         <v>1.1666666666666679</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>39</v>
+      <c r="E3" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4">
+      <c r="A4" s="8">
         <v>44900</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="9">
         <v>0.69444444444444442</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="9">
         <v>0.8125</v>
       </c>
-      <c r="D4" s="3">
-        <f>(C4-B4)*24</f>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
         <v>2.8333333333333339</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5">
-      <c r="A5" s="4">
+      <c r="A5" s="8">
         <v>44901</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="9">
         <v>0.22916666666666666</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="9">
         <v>0.30208333333333331</v>
       </c>
-      <c r="D5" s="3">
-        <f>(C5-B5)*24</f>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
         <v>1.7499999999999998</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6">
-      <c r="A6" s="4">
+      <c r="A6" s="8">
         <v>44901</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="9">
         <v>0.48958333333333331</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="9">
         <v>0.625</v>
       </c>
-      <c r="D6" s="3">
-        <f>(C6-B6)*24</f>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
         <v>3.2500000000000004</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7">
-      <c r="A7" s="4">
+      <c r="A7" s="8">
         <v>44901</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="9">
         <v>0.625</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="9">
         <v>0.64583333333333337</v>
       </c>
-      <c r="D7" s="3">
-        <f>(C7-B7)*24</f>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
         <v>0.50000000000000089</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>40</v>
+      <c r="E7" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4">
+      <c r="A8" s="8">
         <v>44901</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="9">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="9">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D8" s="3">
-        <f>(C8-B8)*24</f>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
         <v>4.0000000000000018</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9">
-      <c r="A9" s="4">
+      <c r="A9" s="8">
         <v>44902</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="9">
         <v>0.25</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="9">
         <v>0.625</v>
       </c>
-      <c r="D9" s="3">
-        <f>(C9-B9)*24</f>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10">
-      <c r="A10" s="4">
+      <c r="A10" s="8">
         <v>44902</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="9">
         <v>0.625</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="9">
         <v>0.78472222222222221</v>
       </c>
-      <c r="D10" s="3">
-        <f>(C10-B10)*24</f>
+      <c r="D10" s="1">
+        <f t="shared" ref="D10:D17" si="1">(C10-B10)*24</f>
         <v>3.833333333333333</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>41</v>
+      <c r="E10" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="4">
+      <c r="A11" s="8">
         <v>44903</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="9">
         <v>0.22916666666666666</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="9">
         <v>0.30208333333333331</v>
       </c>
-      <c r="D11" s="3">
-        <f>(C11-B11)*24</f>
+      <c r="D11" s="1">
+        <f t="shared" si="1"/>
         <v>1.7499999999999998</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="4"/>
     </row>
     <row r="12">
-      <c r="A12" s="4">
+      <c r="A12" s="8">
         <v>44903</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="9">
         <v>0.375</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="9">
         <v>0.55208333333333337</v>
       </c>
-      <c r="D12" s="3">
-        <f>(C12-B12)*24</f>
+      <c r="D12" s="1">
+        <f t="shared" si="1"/>
         <v>4.2500000000000009</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>42</v>
+      <c r="E12" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="4">
+      <c r="A13" s="8">
         <v>44903</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="9">
         <v>0.625</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="9">
         <v>0.81944444444444442</v>
       </c>
-      <c r="D13" s="3">
-        <f>(C13-B13)*24</f>
+      <c r="D13" s="1">
+        <f t="shared" si="1"/>
         <v>4.6666666666666661</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="4"/>
     </row>
     <row r="14">
-      <c r="A14" s="4">
+      <c r="A14" s="8">
         <v>44904</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="9">
         <v>0.22916666666666666</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="9">
         <v>0.3125</v>
       </c>
-      <c r="D14" s="3">
-        <f>(C14-B14)*24</f>
+      <c r="D14" s="1">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15">
-      <c r="A15" s="4">
+      <c r="A15" s="8">
         <v>44904</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="9">
         <v>0.3125</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="9">
         <v>0.82638888888888884</v>
       </c>
-      <c r="D15" s="3">
-        <f>(C15-B15)*24</f>
+      <c r="D15" s="1">
+        <f t="shared" si="1"/>
         <v>12.333333333333332</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>43</v>
+      <c r="E15" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="4">
+      <c r="A16" s="8">
         <v>44905</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="9">
         <v>0.39583333333333331</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="9">
         <v>0.44444444444444442</v>
       </c>
-      <c r="D16" s="3">
-        <f>(C16-B16)*24</f>
+      <c r="D16" s="1">
+        <f t="shared" si="1"/>
         <v>1.1666666666666665</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="4"/>
     </row>
     <row r="17">
-      <c r="A17" s="4">
+      <c r="A17" s="8">
         <v>44905</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="9">
         <v>0.44444444444444442</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="9">
         <v>0.46875</v>
       </c>
-      <c r="D17" s="3">
-        <f>(C17-B17)*24</f>
+      <c r="D17" s="1">
+        <f t="shared" si="1"/>
         <v>0.58333333333333393</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>44</v>
+      <c r="E17" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4">
+      <c r="A18" s="8">
         <v>44906</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="2" t="s">
-        <v>45</v>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="4">
+      <c r="A19" s="8">
         <v>44907</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="2" t="s">
-        <v>46</v>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>